<commit_message>
Waldo Original Experiment data files FINAL
</commit_message>
<xml_diff>
--- a/Data_analysis/Waldo_summer_2019.xlsx
+++ b/Data_analysis/Waldo_summer_2019.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pennychen/Dropbox/waldo_experiment_files/Data_analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE55A66-21E7-054B-8344-BBD4FCDC7372}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1D00FD-FBF5-5846-BBDF-67C48D589878}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="700" windowWidth="33060" windowHeight="16560" xr2:uid="{46280E34-2538-4744-A2CC-A0EC72CC794C}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16560" xr2:uid="{46280E34-2538-4744-A2CC-A0EC72CC794C}"/>
   </bookViews>
   <sheets>
     <sheet name="Experiment" sheetId="2" r:id="rId1"/>
@@ -18,101 +18,6 @@
     <sheet name="Posner_accuracy" sheetId="3" r:id="rId3"/>
     <sheet name="bf_exp" sheetId="1" r:id="rId4"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Experiment!$A$14:$AE$14</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Experiment!$A$15:$AE$15</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Experiment!$A$23:$AE$23</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Experiment!$A$24:$AE$24</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Experiment!$A$25:$AE$25</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Experiment!$A$26:$AE$26</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Experiment!$A$27:$AE$27</definedName>
-    <definedName name="_xlchart.v1.15" hidden="1">Experiment!$A$28:$AE$28</definedName>
-    <definedName name="_xlchart.v1.16" hidden="1">Experiment!$A$29:$AE$29</definedName>
-    <definedName name="_xlchart.v1.17" hidden="1">Experiment!$A$30:$AE$30</definedName>
-    <definedName name="_xlchart.v1.18" hidden="1">Experiment!$A$31:$AE$31</definedName>
-    <definedName name="_xlchart.v1.19" hidden="1">Experiment!$A$32:$AE$32</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Experiment!$A$16:$AE$16</definedName>
-    <definedName name="_xlchart.v1.20" hidden="1">Experiment!$A$33:$AE$33</definedName>
-    <definedName name="_xlchart.v1.21" hidden="1">Experiment!$A$34:$AE$34</definedName>
-    <definedName name="_xlchart.v1.22" hidden="1">Experiment!$A$35:$AE$35</definedName>
-    <definedName name="_xlchart.v1.23" hidden="1">Experiment!$A$36:$AE$36</definedName>
-    <definedName name="_xlchart.v1.24" hidden="1">Experiment!$A$37:$AE$37</definedName>
-    <definedName name="_xlchart.v1.25" hidden="1">Experiment!$A$38:$AE$38</definedName>
-    <definedName name="_xlchart.v1.26" hidden="1">Experiment!$A$39:$AE$39</definedName>
-    <definedName name="_xlchart.v1.27" hidden="1">Experiment!$A$40:$AE$40</definedName>
-    <definedName name="_xlchart.v1.28" hidden="1">Experiment!$A$41:$AE$41</definedName>
-    <definedName name="_xlchart.v1.29" hidden="1">Experiment!$A$42:$AE$42</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Experiment!$A$17:$AE$17</definedName>
-    <definedName name="_xlchart.v1.30" hidden="1">Experiment!$A$43:$AE$43</definedName>
-    <definedName name="_xlchart.v1.31" hidden="1">Experiment!$A$14:$AE$14</definedName>
-    <definedName name="_xlchart.v1.32" hidden="1">Experiment!$A$15:$AE$15</definedName>
-    <definedName name="_xlchart.v1.33" hidden="1">Experiment!$A$16:$AE$16</definedName>
-    <definedName name="_xlchart.v1.34" hidden="1">Experiment!$A$17:$AE$17</definedName>
-    <definedName name="_xlchart.v1.35" hidden="1">Experiment!$A$18:$AE$18</definedName>
-    <definedName name="_xlchart.v1.36" hidden="1">Experiment!$A$19:$AE$19</definedName>
-    <definedName name="_xlchart.v1.37" hidden="1">Experiment!$A$1:$AE$13</definedName>
-    <definedName name="_xlchart.v1.38" hidden="1">Experiment!$A$20:$AE$20</definedName>
-    <definedName name="_xlchart.v1.39" hidden="1">Experiment!$A$21:$AE$21</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Experiment!$A$18:$AE$18</definedName>
-    <definedName name="_xlchart.v1.40" hidden="1">Experiment!$A$22:$AE$22</definedName>
-    <definedName name="_xlchart.v1.41" hidden="1">Experiment!$A$23:$AE$23</definedName>
-    <definedName name="_xlchart.v1.42" hidden="1">Experiment!$A$24:$AE$24</definedName>
-    <definedName name="_xlchart.v1.43" hidden="1">Experiment!$A$25:$AE$25</definedName>
-    <definedName name="_xlchart.v1.44" hidden="1">Experiment!$A$26:$AE$26</definedName>
-    <definedName name="_xlchart.v1.45" hidden="1">Experiment!$A$27:$AE$27</definedName>
-    <definedName name="_xlchart.v1.46" hidden="1">Experiment!$A$28:$AE$28</definedName>
-    <definedName name="_xlchart.v1.47" hidden="1">Experiment!$A$29:$AE$29</definedName>
-    <definedName name="_xlchart.v1.48" hidden="1">Experiment!$A$30:$AE$30</definedName>
-    <definedName name="_xlchart.v1.49" hidden="1">Experiment!$A$31:$AE$31</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Experiment!$A$19:$AE$19</definedName>
-    <definedName name="_xlchart.v1.50" hidden="1">Experiment!$A$32:$AE$32</definedName>
-    <definedName name="_xlchart.v1.51" hidden="1">Experiment!$A$33:$AE$33</definedName>
-    <definedName name="_xlchart.v1.52" hidden="1">Experiment!$A$34:$AE$34</definedName>
-    <definedName name="_xlchart.v1.53" hidden="1">Experiment!$A$35:$AE$35</definedName>
-    <definedName name="_xlchart.v1.54" hidden="1">Experiment!$A$36:$AE$36</definedName>
-    <definedName name="_xlchart.v1.55" hidden="1">Experiment!$A$37:$AE$37</definedName>
-    <definedName name="_xlchart.v1.56" hidden="1">Experiment!$A$38:$AE$38</definedName>
-    <definedName name="_xlchart.v1.57" hidden="1">Experiment!$A$39:$AE$39</definedName>
-    <definedName name="_xlchart.v1.58" hidden="1">Experiment!$A$40:$AE$40</definedName>
-    <definedName name="_xlchart.v1.59" hidden="1">Experiment!$A$41:$AE$41</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Experiment!$A$1:$AE$13</definedName>
-    <definedName name="_xlchart.v1.60" hidden="1">Experiment!$A$42:$AE$42</definedName>
-    <definedName name="_xlchart.v1.61" hidden="1">Experiment!$A$43:$AE$43</definedName>
-    <definedName name="_xlchart.v1.62" hidden="1">Experiment!$A$14:$AE$14</definedName>
-    <definedName name="_xlchart.v1.63" hidden="1">Experiment!$A$15:$AE$15</definedName>
-    <definedName name="_xlchart.v1.64" hidden="1">Experiment!$A$16:$AE$16</definedName>
-    <definedName name="_xlchart.v1.65" hidden="1">Experiment!$A$17:$AE$17</definedName>
-    <definedName name="_xlchart.v1.66" hidden="1">Experiment!$A$18:$AE$18</definedName>
-    <definedName name="_xlchart.v1.67" hidden="1">Experiment!$A$19:$AE$19</definedName>
-    <definedName name="_xlchart.v1.68" hidden="1">Experiment!$A$1:$AE$13</definedName>
-    <definedName name="_xlchart.v1.69" hidden="1">Experiment!$A$20:$AE$20</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Experiment!$A$20:$AE$20</definedName>
-    <definedName name="_xlchart.v1.70" hidden="1">Experiment!$A$21:$AE$21</definedName>
-    <definedName name="_xlchart.v1.71" hidden="1">Experiment!$A$22:$AE$22</definedName>
-    <definedName name="_xlchart.v1.72" hidden="1">Experiment!$A$23:$AE$23</definedName>
-    <definedName name="_xlchart.v1.73" hidden="1">Experiment!$A$24:$AE$24</definedName>
-    <definedName name="_xlchart.v1.74" hidden="1">Experiment!$A$25:$AE$25</definedName>
-    <definedName name="_xlchart.v1.75" hidden="1">Experiment!$A$26:$AE$26</definedName>
-    <definedName name="_xlchart.v1.76" hidden="1">Experiment!$A$27:$AE$27</definedName>
-    <definedName name="_xlchart.v1.77" hidden="1">Experiment!$A$28:$AE$28</definedName>
-    <definedName name="_xlchart.v1.78" hidden="1">Experiment!$A$29:$AE$29</definedName>
-    <definedName name="_xlchart.v1.79" hidden="1">Experiment!$A$30:$AE$30</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Experiment!$A$21:$AE$21</definedName>
-    <definedName name="_xlchart.v1.80" hidden="1">Experiment!$A$31:$AE$31</definedName>
-    <definedName name="_xlchart.v1.81" hidden="1">Experiment!$A$32:$AE$32</definedName>
-    <definedName name="_xlchart.v1.82" hidden="1">Experiment!$A$33:$AE$33</definedName>
-    <definedName name="_xlchart.v1.83" hidden="1">Experiment!$A$34:$AE$34</definedName>
-    <definedName name="_xlchart.v1.84" hidden="1">Experiment!$A$35:$AE$35</definedName>
-    <definedName name="_xlchart.v1.85" hidden="1">Experiment!$A$36:$AE$36</definedName>
-    <definedName name="_xlchart.v1.86" hidden="1">Experiment!$A$37:$AE$37</definedName>
-    <definedName name="_xlchart.v1.87" hidden="1">Experiment!$A$38:$AE$38</definedName>
-    <definedName name="_xlchart.v1.88" hidden="1">Experiment!$A$39:$AE$39</definedName>
-    <definedName name="_xlchart.v1.89" hidden="1">Experiment!$A$40:$AE$40</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Experiment!$A$22:$AE$22</definedName>
-    <definedName name="_xlchart.v1.90" hidden="1">Experiment!$A$41:$AE$41</definedName>
-    <definedName name="_xlchart.v1.91" hidden="1">Experiment!$A$42:$AE$42</definedName>
-    <definedName name="_xlchart.v1.92" hidden="1">Experiment!$A$43:$AE$43</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -121,7 +26,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -713,10 +620,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{455F5E67-AA2D-4341-BE14-B6C3610F182A}">
-  <dimension ref="A1:AE43"/>
+  <dimension ref="A1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="U36" sqref="U36"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1279,7 +1186,7 @@
         <v>0.10878700676717035</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M30" si="9">D6-G6</f>
+        <f t="shared" ref="M6:M29" si="9">D6-G6</f>
         <v>-2.872144604426996E-2</v>
       </c>
       <c r="N6">
@@ -1287,7 +1194,7 @@
         <v>-5.3192669292169814E-2</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O34" si="11">C6-I6</f>
+        <f t="shared" ref="O6:O33" si="11">C6-I6</f>
         <v>2.5983401025470254E-2</v>
       </c>
       <c r="P6">
@@ -3697,7 +3604,7 @@
         <v>0.28573295222896</v>
       </c>
       <c r="M30">
-        <f>D30-G30</f>
+        <f t="shared" ref="M30:M36" si="14">D30-G30</f>
         <v>-0.13719452134938015</v>
       </c>
       <c r="N30">
@@ -3797,7 +3704,7 @@
         <v>0.26798117039725988</v>
       </c>
       <c r="M31">
-        <f>D31-G31</f>
+        <f t="shared" si="14"/>
         <v>0.2032369082793597</v>
       </c>
       <c r="N31">
@@ -3897,7 +3804,7 @@
         <v>9.4143598285460151E-2</v>
       </c>
       <c r="M32">
-        <f>D32-G32</f>
+        <f t="shared" si="14"/>
         <v>-0.1181694821765098</v>
       </c>
       <c r="N32">
@@ -3997,7 +3904,7 @@
         <v>-0.17061365244460003</v>
       </c>
       <c r="M33">
-        <f>D33-G33</f>
+        <f t="shared" si="14"/>
         <v>-0.32922150038442011</v>
       </c>
       <c r="N33">
@@ -4097,7 +4004,7 @@
         <v>0.28557593773612977</v>
       </c>
       <c r="M34">
-        <f>D34-G34</f>
+        <f t="shared" si="14"/>
         <v>-0.30999246803356995</v>
       </c>
       <c r="N34">
@@ -4197,7 +4104,7 @@
         <v>0.23458647180704029</v>
       </c>
       <c r="M35">
-        <f>D35-G35</f>
+        <f t="shared" si="14"/>
         <v>0.29467875258095999</v>
       </c>
       <c r="N35">
@@ -4297,7 +4204,7 @@
         <v>-0.47296046045246998</v>
       </c>
       <c r="M36">
-        <f>D36-G36</f>
+        <f t="shared" si="14"/>
         <v>-0.15620982530526994</v>
       </c>
       <c r="N36">
@@ -4397,7 +4304,7 @@
         <v>-9.1854679644620019E-2</v>
       </c>
       <c r="M37">
-        <f t="shared" ref="M37:M40" si="14">D37-G37</f>
+        <f t="shared" ref="M37:M40" si="15">D37-G37</f>
         <v>0.17581425150009</v>
       </c>
       <c r="N37">
@@ -4405,7 +4312,7 @@
         <v>0.10922042845438007</v>
       </c>
       <c r="O37">
-        <f t="shared" ref="O37:O40" si="15">C37-I37</f>
+        <f t="shared" ref="O37:O40" si="16">C37-I37</f>
         <v>-0.11281486906336013</v>
       </c>
       <c r="P37">
@@ -4497,7 +4404,7 @@
         <v>0.31372649379511008</v>
       </c>
       <c r="M38">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.71198944468198988</v>
       </c>
       <c r="N38">
@@ -4505,7 +4412,7 @@
         <v>-0.52429349725798957</v>
       </c>
       <c r="O38">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>-0.24328093673323981</v>
       </c>
       <c r="P38">
@@ -4597,7 +4504,7 @@
         <v>-0.10401364597371998</v>
       </c>
       <c r="M39">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>5.5310631696229962E-2</v>
       </c>
       <c r="N39">
@@ -4605,7 +4512,7 @@
         <v>-0.65105455088650999</v>
       </c>
       <c r="O39">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>3.0459741052550005E-2</v>
       </c>
       <c r="P39">
@@ -4697,7 +4604,7 @@
         <v>0.16773979767764979</v>
       </c>
       <c r="M40">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>-0.2386810679447402</v>
       </c>
       <c r="N40">
@@ -4705,7 +4612,7 @@
         <v>0.32764480000033025</v>
       </c>
       <c r="O40">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.19851970211847991</v>
       </c>
       <c r="P40">
@@ -4756,21 +4663,6 @@
       </c>
       <c r="AD40">
         <v>1</v>
-      </c>
-    </row>
-    <row r="41" spans="1:30">
-      <c r="A41">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="42" spans="1:30">
-      <c r="A42">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="43" spans="1:30">
-      <c r="A43">
-        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>